<commit_message>
chore: change file name
</commit_message>
<xml_diff>
--- a/0_plan/task.xlsx
+++ b/0_plan/task.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19740" windowHeight="8250" activeTab="1"/>
+    <workbookView windowWidth="19740" windowHeight="8250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sumary" sheetId="4" r:id="rId1"/>
     <sheet name="feature requirement" sheetId="1" r:id="rId2"/>
-    <sheet name="task" sheetId="3" r:id="rId3"/>
+    <sheet name="route analyst" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>link design database mongo</t>
   </si>
@@ -146,7 +146,43 @@
     <t>mỗi role khác nhau sẽ thấy các page khác nhau(frontend)</t>
   </si>
   <si>
-    <t>a</t>
+    <t>route</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>/api/</t>
+  </si>
+  <si>
+    <t>/api-student/</t>
+  </si>
+  <si>
+    <t>/api-teacher/</t>
+  </si>
+  <si>
+    <t>/api/admin/</t>
+  </si>
+  <si>
+    <t>/class-teacher/</t>
+  </si>
+  <si>
+    <t>/class-student/</t>
+  </si>
+  <si>
+    <t>/test-teacher/</t>
+  </si>
+  <si>
+    <t>/test-student/</t>
+  </si>
+  <si>
+    <t>/me</t>
+  </si>
+  <si>
+    <t>/site</t>
+  </si>
+  <si>
+    <t>/chat</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1347,8 @@
   <sheetPr/>
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -1703,17 +1739,81 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="9" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(base): change model, create feature management class for teacher, fix some error with auth
</commit_message>
<xml_diff>
--- a/0_plan/task.xlsx
+++ b/0_plan/task.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19740" windowHeight="8250" activeTab="2"/>
+    <workbookView windowWidth="19740" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="sumary" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>link design database mongo</t>
   </si>
@@ -24,13 +24,16 @@
     <t>https://drawsql.app/teams/anphan/diagrams/education-project</t>
   </si>
   <si>
+    <t>lưu ý: kiểu dữ liệu không giống (xem kỹ hơn tại models tại express)</t>
+  </si>
+  <si>
     <t>Role</t>
   </si>
   <si>
     <t>Page</t>
   </si>
   <si>
-    <t>Describe</t>
+    <t>Describe, navigation page</t>
   </si>
   <si>
     <t>Clone another website</t>
@@ -57,22 +60,16 @@
     <t>các lớp đang tham gia, tìm kiếm và yêu cầu tham gia</t>
   </si>
   <si>
-    <t>Bài kiểm tra</t>
-  </si>
-  <si>
-    <t>page làm bài: (trắc nghiệm, đúng/sai, trả lời ngắn) với chấm điểm tự động.</t>
+    <t>Test page: page làm bài: (trắc nghiệm, đúng/sai, trả lời ngắn) với chấm điểm tự động.</t>
   </si>
   <si>
     <t>page finsh -&gt; hiện số điểm -&gt; số câu đúng -&gt; review lại câu trả lời -&gt; update dữ liệu assignments</t>
   </si>
   <si>
-    <t>Xem video bài giảng với kiểm soát không cho tua.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">page history test </t>
-  </si>
-  <si>
-    <t>Coi lại điểm, review lại những bài test</t>
+    <t>page Xem video bài giảng với kiểm soát không cho tua.</t>
+  </si>
+  <si>
+    <t>Page Coi lại điểm, review lại những bài test</t>
   </si>
   <si>
     <t xml:space="preserve">teacher: </t>
@@ -94,6 +91,9 @@
     <t>page điền đáp án -&gt; redirect đến view bài test</t>
   </si>
   <si>
+    <t>tao assignment video</t>
+  </si>
+  <si>
     <t>Danh sách lớp</t>
   </si>
   <si>
@@ -104,16 +104,10 @@
     <t>page xem điểm của lớp đó, các thông tin khác trong cuộc thi</t>
   </si>
   <si>
-    <t>AI, render file none syntax to syntax</t>
-  </si>
-  <si>
-    <t>difficult feature</t>
-  </si>
-  <si>
     <t xml:space="preserve">admin: </t>
   </si>
   <si>
-    <t>chỉ admin mới được phép set quyền teacher cho user khác</t>
+    <t>set quyền admin, teacher</t>
   </si>
   <si>
     <t>page hiện set quyền teacher cho user yêu cầu</t>
@@ -149,37 +143,31 @@
     <t>route</t>
   </si>
   <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>/api/</t>
-  </si>
-  <si>
-    <t>/api-student/</t>
-  </si>
-  <si>
-    <t>/api-teacher/</t>
-  </si>
-  <si>
-    <t>/api/admin/</t>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>/ will redirect at home-student or home-teacher</t>
+  </si>
+  <si>
+    <t>/home-student/</t>
+  </si>
+  <si>
+    <t>/class-student/</t>
   </si>
   <si>
     <t>/class-teacher/</t>
   </si>
   <si>
-    <t>/class-student/</t>
-  </si>
-  <si>
     <t>/test-teacher/</t>
   </si>
   <si>
-    <t>/test-student/</t>
+    <t>/home-teacher</t>
   </si>
   <si>
     <t>/me</t>
   </si>
   <si>
-    <t>/site</t>
+    <t>/auth</t>
   </si>
   <si>
     <t>/chat</t>
@@ -195,8 +183,16 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
-    <font>
+  <fonts count="24">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -212,118 +208,118 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -386,7 +382,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
+        <fgColor theme="9" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,174 +748,177 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -934,58 +933,61 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1313,24 +1315,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="37.25" customWidth="1"/>
     <col min="2" max="2" width="57.875" customWidth="1"/>
+    <col min="3" max="3" width="50.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1348,378 +1354,372 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="27.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="94" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="31" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="27.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="77.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="31" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E1"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7"/>
       <c r="E2"/>
     </row>
     <row r="3" ht="42.75" spans="1:4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="C4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7"/>
-      <c r="B6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="14"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="18"/>
+      <c r="B19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14" t="s">
+      <c r="C19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" ht="28.5" spans="1:4">
+      <c r="A20" s="18"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" ht="28.5" spans="1:4">
-      <c r="A20" s="16"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="18"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="16"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="17" t="s">
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="18"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" ht="28.5" spans="1:4">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14" t="s">
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" ht="28.5" spans="1:4">
+      <c r="A23" s="18"/>
+      <c r="B23" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="16"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="17" t="s">
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-    </row>
-    <row r="26" ht="28.5" spans="1:4">
-      <c r="A26" s="16"/>
-      <c r="B26" s="15" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="18"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="18"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="18"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="18"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="18"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="21"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="B32" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="15"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="16"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="16"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="16"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="16"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="19"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-    </row>
-    <row r="32" ht="28.5" spans="1:4">
-      <c r="A32" s="20" t="s">
+      <c r="C32" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="D32" s="23"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="24"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="24"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="24"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="24"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="25"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="B38" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="22"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="22"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="22"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="22"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="23"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="24" t="s">
+      <c r="C38" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="D38" s="28"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="29"/>
+      <c r="B39" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C39" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="27"/>
-      <c r="B39" s="26" t="s">
+      <c r="D39" s="28"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="29"/>
+      <c r="B40" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C40" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="27"/>
-      <c r="B40" s="26" t="s">
+      <c r="D40" s="28"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="29"/>
+      <c r="B41" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C41" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="27"/>
-      <c r="B41" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="26"/>
+      <c r="D41" s="28"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="27"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="27"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="27"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="27"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="28"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1741,79 +1741,68 @@
   <sheetPr/>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="9" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="3" max="9" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>42</v>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>